<commit_message>
New MPO file. Report and Deyatelnost modificate
</commit_message>
<xml_diff>
--- a/docs/Deyatelnost.xlsx
+++ b/docs/Deyatelnost.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="n95b9m2wLuvijaFGOPtMs7MBEa6oOSWDKoaCG4TW2bGcGXiU62JvFbrNpzYiWL6bGXOeQFcHthnb6skpENvKKA==" workbookSaltValue="TR9aJ1APSJcF0LfQaM0Haw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Группа" sheetId="1" r:id="rId1"/>
     <sheet name="Проект" sheetId="2" r:id="rId2"/>
-    <sheet name="Инструкции" sheetId="3" r:id="rId3"/>
+    <sheet name="Артефакты" sheetId="4" r:id="rId3"/>
+    <sheet name="Инструкции" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>Дата</t>
   </si>
@@ -249,6 +249,45 @@
   </si>
   <si>
     <t>+50%</t>
+  </si>
+  <si>
+    <t>Наименование артефакта</t>
+  </si>
+  <si>
+    <t>ФИО</t>
+  </si>
+  <si>
+    <t>Действие</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Диаграмма взаимодействия </t>
+  </si>
+  <si>
+    <t>Диаграмма размещения</t>
+  </si>
+  <si>
+    <t>Файл</t>
+  </si>
+  <si>
+    <t>Модель предметной области</t>
+  </si>
+  <si>
+    <t>Варианты использования</t>
+  </si>
+  <si>
+    <t>Зефиров Артём</t>
+  </si>
+  <si>
+    <t>Корректировка</t>
+  </si>
+  <si>
+    <t>tr1_MPO.mdzip</t>
+  </si>
+  <si>
+    <t>tr1.mdzip</t>
+  </si>
+  <si>
+    <t>diagram2_Transas.mdzip</t>
   </si>
 </sst>
 </file>
@@ -372,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -391,9 +430,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -424,14 +460,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -740,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1671,18 +1720,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="B62:B63"/>
     <mergeCell ref="A82:A83"/>
     <mergeCell ref="B82:B83"/>
     <mergeCell ref="A102:A103"/>
     <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1692,350 +1741,350 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="17" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="16" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="19">
         <v>42798</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="19">
         <v>42805</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19">
         <v>42805</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20">
+      <c r="C5" s="18"/>
+      <c r="D5" s="19">
         <v>42805</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20">
+      <c r="C6" s="18"/>
+      <c r="D6" s="19">
         <v>42805</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
         <v>42805</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <v>42805</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="19">
         <v>42812</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="19" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="18" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="19">
         <v>42819</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="19"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="20">
+      <c r="C11" s="12"/>
+      <c r="D11" s="19">
         <v>42826</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="19"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="20">
+      <c r="C12" s="12"/>
+      <c r="D12" s="19">
         <v>42833</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="19"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="19">
         <v>42847</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="19"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="20">
+      <c r="C14" s="12"/>
+      <c r="D14" s="19">
         <v>42812</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="19"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>42819</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="19">
         <v>42826</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="19"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <v>42847</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="19"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="19"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="19">
         <v>42812</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="19"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="19">
         <v>42819</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="19" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="18" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2045,6 +2094,190 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="28">
+        <v>42805</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="28">
+        <v>42805</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="28">
+        <v>42805</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="28">
+        <v>42805</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="28">
+        <v>42805</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="28">
+        <v>42805</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="28">
+        <v>42819</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="28">
+        <v>42819</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2060,10 +2293,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="25"/>
       <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
@@ -2080,7 +2313,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -2091,7 +2324,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="A4" s="22">
         <v>0.75</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -2102,7 +2335,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="A5" s="22">
         <v>0.5</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -2113,7 +2346,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+      <c r="A6" s="22">
         <v>0.25</v>
       </c>
       <c r="B6" s="7" t="s">

</xml_diff>